<commit_message>
Fixed formatting of all files by adding borders and wrap text on header
</commit_message>
<xml_diff>
--- a/FINAL- ALS-CLC 2024 as of May 2025.xlsx
+++ b/FINAL- ALS-CLC 2024 as of May 2025.xlsx
@@ -1,12 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work - Lawrence\Documents\DepEd_scripts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F1D1E4-CCEC-457F-B307-969F3D2D8B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ALS-CLC 2024" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ALS-CLC 2024" sheetId="1" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -28,441 +35,714 @@
     <externalReference r:id="rId18"/>
   </externalReferences>
   <definedNames>
+    <definedName name="\" localSheetId="0">#REF!</definedName>
     <definedName name="\">#REF!</definedName>
+    <definedName name="\a" localSheetId="0">#REF!</definedName>
     <definedName name="\a">#REF!</definedName>
+    <definedName name="\b" localSheetId="0">#REF!</definedName>
     <definedName name="\b">#REF!</definedName>
     <definedName name="\c">#N/A</definedName>
+    <definedName name="___all2" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="___all2" hidden="1">#REF!</definedName>
+    <definedName name="___EDU2" localSheetId="0">[11]EDU4!$G$10</definedName>
     <definedName name="___EDU2">[1]EDU4!$G$10</definedName>
+    <definedName name="__EDU2" localSheetId="0">[11]EDU4!$G$10</definedName>
     <definedName name="__EDU2">[1]EDU4!$G$10</definedName>
+    <definedName name="_all2" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="_all2" hidden="1">#REF!</definedName>
+    <definedName name="_car2" localSheetId="0">#REF!</definedName>
     <definedName name="_car2">#REF!</definedName>
+    <definedName name="_EDU2" localSheetId="0">[11]EDU4!$G$10</definedName>
     <definedName name="_EDU2">[1]EDU4!$G$10</definedName>
+    <definedName name="_Fill" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="_Fill" hidden="1">#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALS-CLC 2024'!$A$1:$W$5</definedName>
+    <definedName name="_Key1" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="_Key1" hidden="1">#REF!</definedName>
+    <definedName name="_Key2" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="_Key2" hidden="1">#REF!</definedName>
     <definedName name="_Order1" hidden="1">255</definedName>
     <definedName name="_Order2" hidden="1">255</definedName>
+    <definedName name="_Sort" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="_Sort" hidden="1">#REF!</definedName>
     <definedName name="_xlcn.WorksheetConnection_BEFF2016A6BV57181">#REF!</definedName>
+    <definedName name="A" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="A">#REF!</definedName>
+    <definedName name="aaaaa" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="aaaaa" hidden="1">#REF!</definedName>
+    <definedName name="ab" localSheetId="0">#REF!</definedName>
     <definedName name="ab">#REF!</definedName>
+    <definedName name="abcd" localSheetId="0">#REF!</definedName>
     <definedName name="abcd">#REF!</definedName>
+    <definedName name="ACCOUNTING" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="ACCOUNTING" hidden="1">#REF!</definedName>
+    <definedName name="adfadfaf" localSheetId="0">#REF!</definedName>
     <definedName name="adfadfaf">#REF!</definedName>
+    <definedName name="ALLREGIONS" localSheetId="0">#REF!</definedName>
     <definedName name="ALLREGIONS">#REF!</definedName>
+    <definedName name="Area" localSheetId="0">#REF!</definedName>
     <definedName name="Area">#REF!</definedName>
+    <definedName name="area2222" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="area2222" hidden="1">#REF!</definedName>
+    <definedName name="asadad" localSheetId="0">#REF!</definedName>
     <definedName name="asadad">#REF!</definedName>
+    <definedName name="ASASDFASFA" localSheetId="0">#REF!</definedName>
     <definedName name="ASASDFASFA">#REF!</definedName>
+    <definedName name="asd" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="asd" hidden="1">#REF!</definedName>
+    <definedName name="ASDAfds" localSheetId="0">#REF!</definedName>
     <definedName name="ASDAfds">#REF!</definedName>
+    <definedName name="ASDFAS" localSheetId="0">#REF!</definedName>
     <definedName name="ASDFAS">#REF!</definedName>
+    <definedName name="awrwqqe" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="awrwqqe" hidden="1">#REF!</definedName>
+    <definedName name="b" localSheetId="0">#REF!</definedName>
     <definedName name="b">#REF!</definedName>
     <definedName name="CLS">[2]Baseline!$1:$1048576</definedName>
+    <definedName name="Cost" localSheetId="0">'[12]Costs and Types'!$A$1:$A$44</definedName>
     <definedName name="Cost">'[3]Costs and Types'!$A$1:$A$44</definedName>
     <definedName name="cv">#REF!</definedName>
+    <definedName name="_xlnm.Database" localSheetId="0">[13]Database!$1:$1048576</definedName>
     <definedName name="_xlnm.Database">[4]Database!$1:$1048576</definedName>
+    <definedName name="dede" localSheetId="0">#REF!</definedName>
     <definedName name="dede">#REF!</definedName>
+    <definedName name="defggr" localSheetId="0">#REF!</definedName>
     <definedName name="defggr">#REF!</definedName>
+    <definedName name="dfre" localSheetId="0">#REF!</definedName>
     <definedName name="dfre">#REF!</definedName>
+    <definedName name="dfsdf" localSheetId="0">#REF!</definedName>
     <definedName name="dfsdf">#REF!</definedName>
+    <definedName name="dfwagagr" localSheetId="0">#REF!</definedName>
     <definedName name="dfwagagr">#REF!</definedName>
+    <definedName name="dsssss" localSheetId="0">#REF!</definedName>
     <definedName name="dsssss">#REF!</definedName>
+    <definedName name="dssssss" localSheetId="0">#REF!</definedName>
     <definedName name="dssssss">#REF!</definedName>
+    <definedName name="e" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="e" hidden="1">#REF!</definedName>
+    <definedName name="ed" localSheetId="0">#REF!</definedName>
     <definedName name="ed">#REF!</definedName>
+    <definedName name="eee" localSheetId="0">#REF!</definedName>
     <definedName name="eee">#REF!</definedName>
+    <definedName name="Eight" localSheetId="0">#REF!</definedName>
     <definedName name="Eight">#REF!</definedName>
+    <definedName name="elem" localSheetId="0">#REF!</definedName>
     <definedName name="elem">#REF!</definedName>
+    <definedName name="enrollment_estimates" localSheetId="0">'[5]Alloc working w formula'!#REF!</definedName>
     <definedName name="enrollment_estimates">'[5]Alloc working w formula'!#REF!</definedName>
+    <definedName name="Enrolment" localSheetId="0">#REF!</definedName>
     <definedName name="Enrolment">#REF!</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_1" localSheetId="0">#REF!</definedName>
     <definedName name="Excel_BuiltIn_Print_Area_1">#REF!</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_3" localSheetId="0">#REF!</definedName>
     <definedName name="Excel_BuiltIn_Print_Area_3">#REF!</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_3_1" localSheetId="0">#REF!</definedName>
     <definedName name="Excel_BuiltIn_Print_Area_3_1">#REF!</definedName>
+    <definedName name="Excel_BuiltIn_Print_Titles_1" localSheetId="0">#REF!</definedName>
     <definedName name="Excel_BuiltIn_Print_Titles_1">#REF!</definedName>
+    <definedName name="exp" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="exp" hidden="1">#REF!</definedName>
+    <definedName name="EXPEND" localSheetId="0">[14]EDU4!$G$10</definedName>
     <definedName name="EXPEND">[6]EDU4!$G$10</definedName>
+    <definedName name="Expenditure" localSheetId="0">#REF!</definedName>
     <definedName name="Expenditure">#REF!</definedName>
+    <definedName name="Expenditure_new" localSheetId="0">#REF!</definedName>
     <definedName name="Expenditure_new">#REF!</definedName>
+    <definedName name="expenditure2" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="expenditure2" hidden="1">#REF!</definedName>
+    <definedName name="F" localSheetId="0">#REF!</definedName>
     <definedName name="F">#REF!</definedName>
+    <definedName name="fift" localSheetId="0">#REF!</definedName>
     <definedName name="fift">#REF!</definedName>
+    <definedName name="Five" localSheetId="0">#REF!</definedName>
     <definedName name="Five">#REF!</definedName>
+    <definedName name="four" localSheetId="0">#REF!</definedName>
     <definedName name="four">#REF!</definedName>
+    <definedName name="gfo" localSheetId="0">[15]Database!$A$3:$E$541</definedName>
     <definedName name="gfo">[7]Database!$A$3:$E$541</definedName>
+    <definedName name="GLEN" localSheetId="0">[16]Database!$A$3:$E$541</definedName>
     <definedName name="GLEN">[8]Database!$A$3:$E$541</definedName>
+    <definedName name="gttt" localSheetId="0">#REF!</definedName>
     <definedName name="gttt">#REF!</definedName>
+    <definedName name="HHHH" localSheetId="0">#REF!</definedName>
     <definedName name="HHHH">#REF!</definedName>
+    <definedName name="hjjhjkj" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="hjjhjkj" hidden="1">#REF!</definedName>
+    <definedName name="I" localSheetId="0">#REF!</definedName>
     <definedName name="I">#REF!</definedName>
+    <definedName name="ie" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="ie" hidden="1">#REF!</definedName>
+    <definedName name="II" localSheetId="0">#REF!</definedName>
     <definedName name="II">#REF!</definedName>
+    <definedName name="III" localSheetId="0">#REF!</definedName>
     <definedName name="III">#REF!</definedName>
+    <definedName name="iree" localSheetId="0">#REF!</definedName>
     <definedName name="iree">#REF!</definedName>
+    <definedName name="IV" localSheetId="0">#REF!</definedName>
     <definedName name="IV">#REF!</definedName>
+    <definedName name="IX" localSheetId="0">#REF!</definedName>
     <definedName name="IX">#REF!</definedName>
+    <definedName name="jik" localSheetId="0">#REF!</definedName>
     <definedName name="jik">#REF!</definedName>
+    <definedName name="jji" localSheetId="0">#REF!</definedName>
     <definedName name="jji">#REF!</definedName>
+    <definedName name="JOEKIM" localSheetId="0">#REF!</definedName>
     <definedName name="JOEKIM">#REF!</definedName>
+    <definedName name="k" localSheetId="0">#REF!</definedName>
     <definedName name="k">#REF!</definedName>
+    <definedName name="kim" localSheetId="0">#REF!</definedName>
     <definedName name="kim">#REF!</definedName>
+    <definedName name="kli" localSheetId="0">#REF!</definedName>
     <definedName name="kli">#REF!</definedName>
+    <definedName name="ko" localSheetId="0">#REF!</definedName>
     <definedName name="ko">#REF!</definedName>
+    <definedName name="l" localSheetId="0">#REF!</definedName>
     <definedName name="l">#REF!</definedName>
+    <definedName name="LCC_WFP" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="LCC_WFP" hidden="1">#REF!</definedName>
+    <definedName name="LCC_WFP2016" localSheetId="0">#REF!</definedName>
     <definedName name="LCC_WFP2016">#REF!</definedName>
+    <definedName name="ll" localSheetId="0">#REF!</definedName>
     <definedName name="ll">#REF!</definedName>
+    <definedName name="llgkih" localSheetId="0">#REF!</definedName>
     <definedName name="llgkih">#REF!</definedName>
+    <definedName name="lll" localSheetId="0">#REF!</definedName>
     <definedName name="lll">#REF!</definedName>
+    <definedName name="m" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="m" hidden="1">#REF!</definedName>
+    <definedName name="marj" localSheetId="0">#REF!</definedName>
     <definedName name="marj">#REF!</definedName>
+    <definedName name="mi" localSheetId="0">#REF!</definedName>
     <definedName name="mi">#REF!</definedName>
+    <definedName name="mial" localSheetId="0">#REF!</definedName>
     <definedName name="mial">#REF!</definedName>
+    <definedName name="mm" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="mm" hidden="1">#REF!</definedName>
+    <definedName name="mmm" localSheetId="0">#REF!</definedName>
     <definedName name="mmm">#REF!</definedName>
+    <definedName name="mmmmmmmmmmmmmm" localSheetId="0">#REF!</definedName>
     <definedName name="mmmmmmmmmmmmmm">#REF!</definedName>
+    <definedName name="mmttr" localSheetId="0">#REF!</definedName>
     <definedName name="mmttr">#REF!</definedName>
+    <definedName name="n" localSheetId="0">#REF!</definedName>
     <definedName name="n">#REF!</definedName>
+    <definedName name="nancy" localSheetId="0">#REF!</definedName>
     <definedName name="nancy">#REF!</definedName>
+    <definedName name="NATIONAL" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="NATIONAL" hidden="1">#REF!</definedName>
+    <definedName name="Natz" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="Natz" hidden="1">#REF!</definedName>
     <definedName name="ncr">#REF!</definedName>
+    <definedName name="new" localSheetId="0">#REF!</definedName>
     <definedName name="new">#REF!</definedName>
+    <definedName name="Nine" localSheetId="0">#REF!</definedName>
     <definedName name="Nine">#REF!</definedName>
+    <definedName name="nnfhfhf" localSheetId="0">#REF!</definedName>
     <definedName name="nnfhfhf">#REF!</definedName>
     <definedName name="NUMCLASS">#N/A</definedName>
+    <definedName name="o" localSheetId="0">#REF!</definedName>
     <definedName name="o">#REF!</definedName>
+    <definedName name="oi" localSheetId="0">#REF!</definedName>
     <definedName name="oi">#REF!</definedName>
+    <definedName name="oldform" localSheetId="0">#REF!</definedName>
     <definedName name="oldform">#REF!</definedName>
+    <definedName name="on" localSheetId="0">#REF!</definedName>
     <definedName name="on">#REF!</definedName>
+    <definedName name="One" localSheetId="0">#REF!</definedName>
     <definedName name="One">#REF!</definedName>
+    <definedName name="oooo" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="oooo" hidden="1">#REF!</definedName>
+    <definedName name="op" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="op" hidden="1">#REF!</definedName>
+    <definedName name="or" localSheetId="0">#REF!</definedName>
     <definedName name="or">#REF!</definedName>
+    <definedName name="Orientation_and_Distribution_of_TXs_TMs__Math_1_2_6___Science_3_6" localSheetId="0">#REF!</definedName>
     <definedName name="Orientation_and_Distribution_of_TXs_TMs__Math_1_2_6___Science_3_6">#REF!</definedName>
+    <definedName name="p" localSheetId="0">#REF!</definedName>
     <definedName name="p">#REF!</definedName>
+    <definedName name="po" localSheetId="0">#REF!</definedName>
     <definedName name="po">#REF!</definedName>
+    <definedName name="ppmp_01" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="ppmp_01" hidden="1">#REF!</definedName>
+    <definedName name="PPMP1" localSheetId="0">#REF!</definedName>
     <definedName name="PPMP1">#REF!</definedName>
+    <definedName name="ppmp2" localSheetId="0">#REF!</definedName>
     <definedName name="ppmp2">#REF!</definedName>
+    <definedName name="Prin" localSheetId="0">#REF!</definedName>
     <definedName name="Prin">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'ALS-CLC 2024'!$A$1:$I$5</definedName>
+    <definedName name="PRINT_AREA_MI" localSheetId="0">#REF!</definedName>
     <definedName name="PRINT_AREA_MI">#REF!</definedName>
+    <definedName name="print_area_Mil" localSheetId="0">#REF!</definedName>
     <definedName name="print_area_Mil">#REF!</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'ALS-CLC 2024'!$1:$1</definedName>
+    <definedName name="Print_Titles_MI" localSheetId="0">'[17]Enrolees&amp;Graduated'!$A$1:$IV$6,'[17]Enrolees&amp;Graduated'!$A$1:$A$65536</definedName>
     <definedName name="Print_Titles_MI">'[9]Enrolees&amp;Graduated'!$A$1:$IV$6,'[9]Enrolees&amp;Graduated'!$A$1:$A$65536</definedName>
+    <definedName name="procured" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="procured" hidden="1">#REF!</definedName>
+    <definedName name="Procurement" localSheetId="0">#REF!</definedName>
     <definedName name="Procurement">#REF!</definedName>
+    <definedName name="py" localSheetId="0">#REF!</definedName>
     <definedName name="py">#REF!</definedName>
+    <definedName name="q" localSheetId="0">#REF!</definedName>
     <definedName name="q">#REF!</definedName>
+    <definedName name="reg" localSheetId="0">#REF!</definedName>
     <definedName name="reg">#REF!</definedName>
+    <definedName name="region" localSheetId="0">#REF!</definedName>
     <definedName name="region">#REF!</definedName>
+    <definedName name="Region2" localSheetId="0">#REF!</definedName>
     <definedName name="Region2">#REF!</definedName>
+    <definedName name="regional" localSheetId="0">#REF!</definedName>
     <definedName name="regional">#REF!</definedName>
+    <definedName name="ret" localSheetId="0">#REF!</definedName>
     <definedName name="ret">#REF!</definedName>
+    <definedName name="ro" localSheetId="0">#REF!</definedName>
     <definedName name="ro">#REF!</definedName>
+    <definedName name="rommel" localSheetId="0">#REF!</definedName>
     <definedName name="rommel">#REF!</definedName>
+    <definedName name="rrr" localSheetId="0">#REF!</definedName>
     <definedName name="rrr">#REF!</definedName>
+    <definedName name="RSBP" localSheetId="0">#REF!</definedName>
     <definedName name="RSBP">#REF!</definedName>
+    <definedName name="safe" localSheetId="0">[10]SchInfo!#REF!</definedName>
     <definedName name="safe">[10]SchInfo!#REF!</definedName>
+    <definedName name="sayot" localSheetId="0">#REF!</definedName>
     <definedName name="sayot">#REF!</definedName>
+    <definedName name="seco" localSheetId="0">#REF!</definedName>
     <definedName name="seco">#REF!</definedName>
+    <definedName name="sed" localSheetId="0">#REF!</definedName>
     <definedName name="sed">#REF!</definedName>
+    <definedName name="sev" localSheetId="0">#REF!</definedName>
     <definedName name="sev">#REF!</definedName>
+    <definedName name="Seven" localSheetId="0">#REF!</definedName>
     <definedName name="Seven">#REF!</definedName>
+    <definedName name="sheet" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="sheet" hidden="1">#REF!</definedName>
+    <definedName name="shsid2" localSheetId="0">#REF!</definedName>
     <definedName name="shsid2">#REF!</definedName>
+    <definedName name="six" localSheetId="0">#REF!</definedName>
     <definedName name="six">#REF!</definedName>
     <definedName name="Slicer_CATEGORY">#REF!</definedName>
     <definedName name="Slicer_CATEGORY1">#REF!</definedName>
     <definedName name="Slicer_REGION">#REF!</definedName>
     <definedName name="Slicer_REGION1">#REF!</definedName>
+    <definedName name="Soil_Condition" localSheetId="0">#REF!</definedName>
     <definedName name="Soil_Condition">#REF!</definedName>
+    <definedName name="sss" localSheetId="0">#REF!</definedName>
     <definedName name="sss">#REF!</definedName>
+    <definedName name="SUMM2016VER2" localSheetId="0">#REF!</definedName>
     <definedName name="SUMM2016VER2">#REF!</definedName>
+    <definedName name="Table_13" localSheetId="0">#REF!</definedName>
     <definedName name="Table_13">#REF!</definedName>
+    <definedName name="Table_14" localSheetId="0">#REF!</definedName>
     <definedName name="Table_14">#REF!</definedName>
+    <definedName name="Table_15" localSheetId="0">#REF!</definedName>
     <definedName name="Table_15">#REF!</definedName>
+    <definedName name="Table_18" localSheetId="0">#REF!</definedName>
     <definedName name="Table_18">#REF!</definedName>
+    <definedName name="Table_19" localSheetId="0">#REF!</definedName>
     <definedName name="Table_19">#REF!</definedName>
+    <definedName name="Table19" localSheetId="0">#REF!</definedName>
     <definedName name="Table19">#REF!</definedName>
+    <definedName name="Th" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="Th" hidden="1">#REF!</definedName>
+    <definedName name="three" localSheetId="0">#REF!</definedName>
     <definedName name="three">#REF!</definedName>
+    <definedName name="to" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="to" hidden="1">#REF!</definedName>
+    <definedName name="tree" localSheetId="0">#REF!</definedName>
     <definedName name="tree">#REF!</definedName>
+    <definedName name="TS" localSheetId="0">#REF!</definedName>
     <definedName name="TS">#REF!</definedName>
+    <definedName name="Twelve" localSheetId="0">#REF!</definedName>
     <definedName name="Twelve">#REF!</definedName>
+    <definedName name="two" localSheetId="0">#REF!</definedName>
     <definedName name="two">#REF!</definedName>
+    <definedName name="ty" localSheetId="0">#REF!</definedName>
     <definedName name="ty">#REF!</definedName>
+    <definedName name="V" localSheetId="0">#REF!</definedName>
     <definedName name="V">#REF!</definedName>
+    <definedName name="VI" localSheetId="0">#REF!</definedName>
     <definedName name="VI">#REF!</definedName>
+    <definedName name="VIII" localSheetId="0">#REF!</definedName>
     <definedName name="VIII">#REF!</definedName>
+    <definedName name="VIIII" localSheetId="0">#REF!</definedName>
     <definedName name="VIIII">#REF!</definedName>
+    <definedName name="WDAFA" localSheetId="0">#REF!</definedName>
     <definedName name="WDAFA">#REF!</definedName>
+    <definedName name="wdf" localSheetId="0">#REF!</definedName>
     <definedName name="wdf">#REF!</definedName>
+    <definedName name="wfdp" localSheetId="0">#REF!</definedName>
     <definedName name="wfdp">#REF!</definedName>
+    <definedName name="WFP" localSheetId="0">#REF!</definedName>
     <definedName name="WFP">#REF!</definedName>
+    <definedName name="wp" localSheetId="0">#REF!</definedName>
     <definedName name="wp">#REF!</definedName>
+    <definedName name="X" localSheetId="0">#REF!</definedName>
     <definedName name="X">#REF!</definedName>
+    <definedName name="XXX" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="XXX" hidden="1">#REF!</definedName>
+    <definedName name="y" localSheetId="0">#REF!</definedName>
     <definedName name="y">#REF!</definedName>
+    <definedName name="yh" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="yh" hidden="1">#REF!</definedName>
+    <definedName name="yolanda" localSheetId="0">#REF!</definedName>
     <definedName name="yolanda">#REF!</definedName>
+    <definedName name="yt" localSheetId="0">#REF!</definedName>
     <definedName name="yt">#REF!</definedName>
+    <definedName name="zero" localSheetId="0">#REF!</definedName>
     <definedName name="zero">#REF!</definedName>
-    <definedName name="\" localSheetId="0">#REF!</definedName>
-    <definedName name="\a" localSheetId="0">#REF!</definedName>
-    <definedName name="\b" localSheetId="0">#REF!</definedName>
-    <definedName name="___all2" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="___EDU2" localSheetId="0">[11]EDU4!$G$10</definedName>
-    <definedName name="__EDU2" localSheetId="0">[11]EDU4!$G$10</definedName>
-    <definedName name="_all2" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="_car2" localSheetId="0">#REF!</definedName>
-    <definedName name="_EDU2" localSheetId="0">[11]EDU4!$G$10</definedName>
-    <definedName name="_Fill" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="_Key1" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="_Key2" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="_Sort" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="A" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="aaaaa" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="ab" localSheetId="0">#REF!</definedName>
-    <definedName name="abcd" localSheetId="0">#REF!</definedName>
-    <definedName name="ACCOUNTING" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="adfadfaf" localSheetId="0">#REF!</definedName>
-    <definedName name="ALLREGIONS" localSheetId="0">#REF!</definedName>
-    <definedName name="Area" localSheetId="0">#REF!</definedName>
-    <definedName name="area2222" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="asadad" localSheetId="0">#REF!</definedName>
-    <definedName name="ASASDFASFA" localSheetId="0">#REF!</definedName>
-    <definedName name="asd" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="ASDAfds" localSheetId="0">#REF!</definedName>
-    <definedName name="ASDFAS" localSheetId="0">#REF!</definedName>
-    <definedName name="awrwqqe" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="b" localSheetId="0">#REF!</definedName>
-    <definedName name="Cost" localSheetId="0">'[12]Costs and Types'!$A$1:$A$44</definedName>
-    <definedName name="_xlnm.Database" localSheetId="0">[13]Database!$1:$1048576</definedName>
-    <definedName name="dede" localSheetId="0">#REF!</definedName>
-    <definedName name="defggr" localSheetId="0">#REF!</definedName>
-    <definedName name="dfre" localSheetId="0">#REF!</definedName>
-    <definedName name="dfsdf" localSheetId="0">#REF!</definedName>
-    <definedName name="dfwagagr" localSheetId="0">#REF!</definedName>
-    <definedName name="dsssss" localSheetId="0">#REF!</definedName>
-    <definedName name="dssssss" localSheetId="0">#REF!</definedName>
-    <definedName name="e" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="ed" localSheetId="0">#REF!</definedName>
-    <definedName name="eee" localSheetId="0">#REF!</definedName>
-    <definedName name="Eight" localSheetId="0">#REF!</definedName>
-    <definedName name="elem" localSheetId="0">#REF!</definedName>
-    <definedName name="enrollment_estimates" localSheetId="0">'[5]Alloc working w formula'!#REF!</definedName>
-    <definedName name="Enrolment" localSheetId="0">#REF!</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area_1" localSheetId="0">#REF!</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area_3" localSheetId="0">#REF!</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area_3_1" localSheetId="0">#REF!</definedName>
-    <definedName name="Excel_BuiltIn_Print_Titles_1" localSheetId="0">#REF!</definedName>
-    <definedName name="exp" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="EXPEND" localSheetId="0">[14]EDU4!$G$10</definedName>
-    <definedName name="Expenditure" localSheetId="0">#REF!</definedName>
-    <definedName name="Expenditure_new" localSheetId="0">#REF!</definedName>
-    <definedName name="expenditure2" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="F" localSheetId="0">#REF!</definedName>
-    <definedName name="fift" localSheetId="0">#REF!</definedName>
-    <definedName name="Five" localSheetId="0">#REF!</definedName>
-    <definedName name="four" localSheetId="0">#REF!</definedName>
-    <definedName name="gfo" localSheetId="0">[15]Database!$A$3:$E$541</definedName>
-    <definedName name="GLEN" localSheetId="0">[16]Database!$A$3:$E$541</definedName>
-    <definedName name="gttt" localSheetId="0">#REF!</definedName>
-    <definedName name="HHHH" localSheetId="0">#REF!</definedName>
-    <definedName name="hjjhjkj" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="I" localSheetId="0">#REF!</definedName>
-    <definedName name="ie" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="II" localSheetId="0">#REF!</definedName>
-    <definedName name="III" localSheetId="0">#REF!</definedName>
-    <definedName name="iree" localSheetId="0">#REF!</definedName>
-    <definedName name="IV" localSheetId="0">#REF!</definedName>
-    <definedName name="IX" localSheetId="0">#REF!</definedName>
-    <definedName name="jik" localSheetId="0">#REF!</definedName>
-    <definedName name="jji" localSheetId="0">#REF!</definedName>
-    <definedName name="JOEKIM" localSheetId="0">#REF!</definedName>
-    <definedName name="k" localSheetId="0">#REF!</definedName>
-    <definedName name="kim" localSheetId="0">#REF!</definedName>
-    <definedName name="kli" localSheetId="0">#REF!</definedName>
-    <definedName name="ko" localSheetId="0">#REF!</definedName>
-    <definedName name="l" localSheetId="0">#REF!</definedName>
-    <definedName name="LCC_WFP" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="LCC_WFP2016" localSheetId="0">#REF!</definedName>
-    <definedName name="ll" localSheetId="0">#REF!</definedName>
-    <definedName name="llgkih" localSheetId="0">#REF!</definedName>
-    <definedName name="lll" localSheetId="0">#REF!</definedName>
-    <definedName name="m" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="marj" localSheetId="0">#REF!</definedName>
-    <definedName name="mi" localSheetId="0">#REF!</definedName>
-    <definedName name="mial" localSheetId="0">#REF!</definedName>
-    <definedName name="mm" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="mmm" localSheetId="0">#REF!</definedName>
-    <definedName name="mmmmmmmmmmmmmm" localSheetId="0">#REF!</definedName>
-    <definedName name="mmttr" localSheetId="0">#REF!</definedName>
-    <definedName name="n" localSheetId="0">#REF!</definedName>
-    <definedName name="nancy" localSheetId="0">#REF!</definedName>
-    <definedName name="NATIONAL" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="Natz" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="new" localSheetId="0">#REF!</definedName>
-    <definedName name="Nine" localSheetId="0">#REF!</definedName>
-    <definedName name="nnfhfhf" localSheetId="0">#REF!</definedName>
-    <definedName name="o" localSheetId="0">#REF!</definedName>
-    <definedName name="oi" localSheetId="0">#REF!</definedName>
-    <definedName name="oldform" localSheetId="0">#REF!</definedName>
-    <definedName name="on" localSheetId="0">#REF!</definedName>
-    <definedName name="One" localSheetId="0">#REF!</definedName>
-    <definedName name="oooo" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="op" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="or" localSheetId="0">#REF!</definedName>
-    <definedName name="Orientation_and_Distribution_of_TXs_TMs__Math_1_2_6___Science_3_6" localSheetId="0">#REF!</definedName>
-    <definedName name="p" localSheetId="0">#REF!</definedName>
-    <definedName name="po" localSheetId="0">#REF!</definedName>
-    <definedName name="ppmp_01" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="PPMP1" localSheetId="0">#REF!</definedName>
-    <definedName name="ppmp2" localSheetId="0">#REF!</definedName>
-    <definedName name="Prin" localSheetId="0">#REF!</definedName>
-    <definedName name="PRINT_AREA_MI" localSheetId="0">#REF!</definedName>
-    <definedName name="print_area_Mil" localSheetId="0">#REF!</definedName>
-    <definedName name="Print_Titles_MI" localSheetId="0">'[17]Enrolees&amp;Graduated'!$A$1:$IV$6,'[17]Enrolees&amp;Graduated'!$A$1:$A$65536</definedName>
-    <definedName name="procured" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="Procurement" localSheetId="0">#REF!</definedName>
-    <definedName name="py" localSheetId="0">#REF!</definedName>
-    <definedName name="q" localSheetId="0">#REF!</definedName>
-    <definedName name="reg" localSheetId="0">#REF!</definedName>
-    <definedName name="region" localSheetId="0">#REF!</definedName>
-    <definedName name="Region2" localSheetId="0">#REF!</definedName>
-    <definedName name="regional" localSheetId="0">#REF!</definedName>
-    <definedName name="ret" localSheetId="0">#REF!</definedName>
-    <definedName name="ro" localSheetId="0">#REF!</definedName>
-    <definedName name="rommel" localSheetId="0">#REF!</definedName>
-    <definedName name="rrr" localSheetId="0">#REF!</definedName>
-    <definedName name="RSBP" localSheetId="0">#REF!</definedName>
-    <definedName name="safe" localSheetId="0">[10]SchInfo!#REF!</definedName>
-    <definedName name="sayot" localSheetId="0">#REF!</definedName>
-    <definedName name="seco" localSheetId="0">#REF!</definedName>
-    <definedName name="sed" localSheetId="0">#REF!</definedName>
-    <definedName name="sev" localSheetId="0">#REF!</definedName>
-    <definedName name="Seven" localSheetId="0">#REF!</definedName>
-    <definedName name="sheet" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="shsid2" localSheetId="0">#REF!</definedName>
-    <definedName name="six" localSheetId="0">#REF!</definedName>
-    <definedName name="Soil_Condition" localSheetId="0">#REF!</definedName>
-    <definedName name="sss" localSheetId="0">#REF!</definedName>
-    <definedName name="SUMM2016VER2" localSheetId="0">#REF!</definedName>
-    <definedName name="Table_13" localSheetId="0">#REF!</definedName>
-    <definedName name="Table_14" localSheetId="0">#REF!</definedName>
-    <definedName name="Table_15" localSheetId="0">#REF!</definedName>
-    <definedName name="Table_18" localSheetId="0">#REF!</definedName>
-    <definedName name="Table_19" localSheetId="0">#REF!</definedName>
-    <definedName name="Table19" localSheetId="0">#REF!</definedName>
-    <definedName name="Th" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="three" localSheetId="0">#REF!</definedName>
-    <definedName name="to" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="tree" localSheetId="0">#REF!</definedName>
-    <definedName name="TS" localSheetId="0">#REF!</definedName>
-    <definedName name="Twelve" localSheetId="0">#REF!</definedName>
-    <definedName name="two" localSheetId="0">#REF!</definedName>
-    <definedName name="ty" localSheetId="0">#REF!</definedName>
-    <definedName name="V" localSheetId="0">#REF!</definedName>
-    <definedName name="VI" localSheetId="0">#REF!</definedName>
-    <definedName name="VIII" localSheetId="0">#REF!</definedName>
-    <definedName name="VIIII" localSheetId="0">#REF!</definedName>
-    <definedName name="WDAFA" localSheetId="0">#REF!</definedName>
-    <definedName name="wdf" localSheetId="0">#REF!</definedName>
-    <definedName name="wfdp" localSheetId="0">#REF!</definedName>
-    <definedName name="WFP" localSheetId="0">#REF!</definedName>
-    <definedName name="wp" localSheetId="0">#REF!</definedName>
-    <definedName name="X" localSheetId="0">#REF!</definedName>
-    <definedName name="XXX" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="y" localSheetId="0">#REF!</definedName>
-    <definedName name="yh" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="yolanda" localSheetId="0">#REF!</definedName>
-    <definedName name="yt" localSheetId="0">#REF!</definedName>
-    <definedName name="zero" localSheetId="0">#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALS-CLC 2024'!$A$1:$AI$5</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'ALS-CLC 2024'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'ALS-CLC 2024'!$A$1:$I$5</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>School ID</t>
+  </si>
+  <si>
+    <t>School Name</t>
+  </si>
+  <si>
+    <t>Municipality</t>
+  </si>
+  <si>
+    <t>Leg District</t>
+  </si>
+  <si>
+    <t>No. of Sites</t>
+  </si>
+  <si>
+    <t>Scope of Work</t>
+  </si>
+  <si>
+    <t>Total Allocation</t>
+  </si>
+  <si>
+    <t>CONTRACT AMOUNT</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>PERCENTAGE OF COMPLETION</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Target Completion Date </t>
+  </si>
+  <si>
+    <t>Actual Date of Completion</t>
+  </si>
+  <si>
+    <t>Project ID</t>
+  </si>
+  <si>
+    <t>Contract ID</t>
+  </si>
+  <si>
+    <t>Issuance of Invitation to Bid</t>
+  </si>
+  <si>
+    <t>Pre-Submission Conference</t>
+  </si>
+  <si>
+    <t>Bid Opening</t>
+  </si>
+  <si>
+    <t>Issuance of Resolution to Award</t>
+  </si>
+  <si>
+    <t>Issuance of Notice to Proceed</t>
+  </si>
+  <si>
+    <t>Name of Contractor</t>
+  </si>
+  <si>
+    <t>Other Remarks</t>
+  </si>
+  <si>
+    <t>CARAGA</t>
+  </si>
+  <si>
+    <t>Agusan del Norte</t>
+  </si>
+  <si>
+    <t>Buenavista CES</t>
+  </si>
+  <si>
+    <t>BUENAVISTA</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>CONSTRUCTION OF TWO (2) STOREY ALTERNATIVE LEARNING SYSTEM - COMMUNITY LEARNING CENTER WITH ROOF DECK- (18.00m x 9.50m), WITH RAINWATER COLLECTOR, PERIMETER FENCE AND FURNITURE</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>April 26, 2025</t>
+  </si>
+  <si>
+    <t>May 15, 2025</t>
+  </si>
+  <si>
+    <t>ALS-CLC 2024 - CARAGA - AGUSAN DEL NORTE - 001</t>
+  </si>
+  <si>
+    <t>June 5, 2024</t>
+  </si>
+  <si>
+    <t>June 28, 2024</t>
+  </si>
+  <si>
+    <t>July 11, 2024</t>
+  </si>
+  <si>
+    <t>August 5, 2024</t>
+  </si>
+  <si>
+    <t>August 15, 2024</t>
+  </si>
+  <si>
+    <t>JD-RG Const. &amp; Supplies</t>
+  </si>
+  <si>
+    <t>WITH VARIATION ORDER AND TIME EXTENSION</t>
+  </si>
+  <si>
+    <t>Region I</t>
+  </si>
+  <si>
+    <t>Ilocos Sur</t>
+  </si>
+  <si>
+    <t>Sta. Cruz CS</t>
+  </si>
+  <si>
+    <t>SANTA CRUZ</t>
+  </si>
+  <si>
+    <t>PROPOSED TWO (2) - STOREY ALTERNATIVE LEARNING SYSTEM (ALS) BUILDING (22.50m x 9.50m) - with Roof Deck</t>
+  </si>
+  <si>
+    <t>Original: 9,322,239.10
+Revised: Php 10,250,272.33</t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <t>Original: 4/18/2025
+Revised: 5/18/2025</t>
+  </si>
+  <si>
+    <t>PB-015-2024</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>October 2, 2024</t>
+  </si>
+  <si>
+    <t>October 9, 2024</t>
+  </si>
+  <si>
+    <t>October 22, 2024</t>
+  </si>
+  <si>
+    <t>October 30, 2024</t>
+  </si>
+  <si>
+    <t>November 20, 2024</t>
+  </si>
+  <si>
+    <t>MA Tejada COnstruction</t>
+  </si>
+  <si>
+    <t>With additional works amounting to Php 928,033.23 due to revision of plans</t>
+  </si>
+  <si>
+    <t>Region III</t>
+  </si>
+  <si>
+    <t>Aurora</t>
+  </si>
+  <si>
+    <t>Lual NHS</t>
+  </si>
+  <si>
+    <t>CASIGURAN</t>
+  </si>
+  <si>
+    <t>Lone</t>
+  </si>
+  <si>
+    <t>PROPOSED TWO (2) - STOREY ALTERNATIVE LEARNING SYSTEM (ALS) BUILDING (22.50m x 9.50m) - with Roof Deck( TO be elevated by 1.0m)</t>
+  </si>
+  <si>
+    <t>June 21, 2025</t>
+  </si>
+  <si>
+    <t>2024-04-181</t>
+  </si>
+  <si>
+    <t>SGOD-INFRA-32</t>
+  </si>
+  <si>
+    <t>July 1, 2024</t>
+  </si>
+  <si>
+    <t>July 8, 2024</t>
+  </si>
+  <si>
+    <t>July 22, 2024</t>
+  </si>
+  <si>
+    <t>August 1, 2024</t>
+  </si>
+  <si>
+    <t>August 17, 2024</t>
+  </si>
+  <si>
+    <t>MACCO CONSTRUCTION</t>
+  </si>
+  <si>
+    <t>Request to utilized savings is up to now no response from CO</t>
+  </si>
+  <si>
+    <t>Region IV-B</t>
+  </si>
+  <si>
+    <t>Occidental Mindoro</t>
+  </si>
+  <si>
+    <t>Sablayan National Comprehensive High School</t>
+  </si>
+  <si>
+    <t>SABLAYAN</t>
+  </si>
+  <si>
+    <t>April 10, 2025</t>
+  </si>
+  <si>
+    <t>April 15,2025</t>
+  </si>
+  <si>
+    <t>DepEd-OccMdo-2024-05</t>
+  </si>
+  <si>
+    <t>May 31, 2024</t>
+  </si>
+  <si>
+    <t>June 10 2024</t>
+  </si>
+  <si>
+    <t>June 24, 2024</t>
+  </si>
+  <si>
+    <t>June 19, 2024</t>
+  </si>
+  <si>
+    <t>hawkstow construction and development</t>
+  </si>
+  <si>
+    <t>actual target completion was adjusted due to contractor request for extension regarding weather condition</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <sz val="12"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.7999816888943144"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -470,18 +750,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor rgb="FFFFC000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFD6DCE4"/>
       </patternFill>
     </fill>
   </fills>
@@ -534,102 +802,80 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="22">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf numFmtId="43" fontId="3" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="5">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal 2 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 41" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
-    <cellStyle name="Comma 2" xfId="3"/>
-    <cellStyle name="Normal 41" xfId="4"/>
-    <cellStyle name="Normal 2 2 2" xfId="5"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.3999450666829432"/>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -665,80 +911,20 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="EDU4"/>
       <sheetName val="edu May -ot"/>
@@ -768,8 +954,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="SchInfo"/>
       <sheetName val="Table1"/>
@@ -833,8 +1019,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="EDU4"/>
       <sheetName val="edu May -ot"/>
@@ -868,8 +1054,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="PRIORITY 2"/>
       <sheetName val="PRIORITY 3"/>
@@ -887,8 +1073,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Liminangcong"/>
       <sheetName val="Recommendation"/>
@@ -2466,8 +2652,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="EDU4"/>
       <sheetName val="edu May -ot"/>
@@ -2497,8 +2683,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="summary"/>
       <sheetName val="Graceano Lopez"/>
@@ -4200,8 +4386,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="POW"/>
       <sheetName val="Lupang Pangako"/>
@@ -4281,8 +4467,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Enrolees&amp;Graduated"/>
       <sheetName val="Classrooms"/>
@@ -4300,8 +4486,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="REGIONS AND DIVISIONS"/>
       <sheetName val="Sheet1"/>
@@ -4325,8 +4511,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="PRIORITY 2"/>
       <sheetName val="PRIORITY 3"/>
@@ -4344,8 +4530,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Liminangcong"/>
       <sheetName val="Recommendation"/>
@@ -6267,8 +6453,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="for DBM"/>
       <sheetName val="FINAL ALLOCATION"/>
@@ -6302,8 +6488,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="EDU4"/>
       <sheetName val="edu May -ot"/>
@@ -6331,8 +6517,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="summary"/>
       <sheetName val="Graceano Lopez"/>
@@ -6460,8 +6646,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="POW"/>
       <sheetName val="Lupang Pangako"/>
@@ -6593,8 +6779,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Enrolees&amp;Graduated"/>
       <sheetName val="Classrooms"/>
@@ -6905,794 +7091,408 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D18" sqref="D18:D19"/>
       <selection pane="bottomLeft" activeCell="D18" sqref="D18:D19"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col width="19.26953125" customWidth="1" style="1" min="1" max="1"/>
-    <col width="29" customWidth="1" style="1" min="2" max="2"/>
-    <col width="14.81640625" customWidth="1" style="1" min="3" max="3"/>
-    <col width="35.26953125" customWidth="1" style="1" min="4" max="4"/>
-    <col width="32.453125" customWidth="1" style="1" min="5" max="5"/>
-    <col width="9.7265625" customWidth="1" style="1" min="6" max="6"/>
-    <col width="10.453125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="29.453125" customWidth="1" style="1" min="8" max="8"/>
-    <col width="36" customWidth="1" style="19" min="9" max="9"/>
-    <col width="16.81640625" customWidth="1" style="3" min="10" max="10"/>
-    <col width="16.81640625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="16.81640625" customWidth="1" style="4" min="12" max="12"/>
-    <col width="16.81640625" customWidth="1" style="5" min="13" max="14"/>
-    <col width="16.81640625" customWidth="1" style="1" min="15" max="16"/>
-    <col width="16.81640625" customWidth="1" style="5" min="17" max="20"/>
-    <col width="29.54296875" customWidth="1" style="5" min="21" max="21"/>
-    <col width="16.81640625" customWidth="1" style="1" min="22" max="23"/>
-    <col width="9.1796875" customWidth="1" style="1" min="24" max="32"/>
-    <col width="17.453125" customWidth="1" style="1" min="33" max="33"/>
-    <col width="9.1796875" customWidth="1" style="1" min="34" max="34"/>
-    <col width="9.1796875" customWidth="1" style="1" min="35" max="16384"/>
+    <col min="1" max="1" width="19.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="29.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="36" style="15" customWidth="1"/>
+    <col min="10" max="10" width="16.81640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.81640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" style="4" customWidth="1"/>
+    <col min="13" max="14" width="16.81640625" style="5" customWidth="1"/>
+    <col min="15" max="16" width="16.81640625" style="1" customWidth="1"/>
+    <col min="17" max="20" width="16.81640625" style="5" customWidth="1"/>
+    <col min="21" max="21" width="29.54296875" style="5" customWidth="1"/>
+    <col min="22" max="23" width="16.81640625" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="60.65" customFormat="1" customHeight="1" s="16">
-      <c r="A1" s="6" t="inlineStr">
-        <is>
-          <t>Region</t>
-        </is>
-      </c>
-      <c r="B1" s="6" t="inlineStr">
-        <is>
-          <t>Division</t>
-        </is>
-      </c>
-      <c r="C1" s="6" t="inlineStr">
-        <is>
-          <t>School ID</t>
-        </is>
-      </c>
-      <c r="D1" s="6" t="inlineStr">
-        <is>
-          <t>School Name</t>
-        </is>
-      </c>
-      <c r="E1" s="6" t="inlineStr">
-        <is>
-          <t>Municipality</t>
-        </is>
-      </c>
-      <c r="F1" s="6" t="inlineStr">
-        <is>
-          <t>Leg District</t>
-        </is>
-      </c>
-      <c r="G1" s="7" t="inlineStr">
-        <is>
-          <t>No. of Sites</t>
-        </is>
-      </c>
-      <c r="H1" s="6" t="inlineStr">
-        <is>
-          <t>Scope of Work</t>
-        </is>
-      </c>
-      <c r="I1" s="8" t="inlineStr">
-        <is>
-          <t>Total Allocation</t>
-        </is>
-      </c>
-      <c r="J1" s="9" t="inlineStr">
-        <is>
-          <t>CONTRACT AMOUNT</t>
-        </is>
-      </c>
-      <c r="K1" s="10" t="inlineStr">
-        <is>
-          <t>STATUS</t>
-        </is>
-      </c>
-      <c r="L1" s="11" t="inlineStr">
-        <is>
-          <t>PERCENTAGE OF COMPLETION</t>
-        </is>
-      </c>
-      <c r="M1" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Target Completion Date </t>
-        </is>
-      </c>
-      <c r="N1" s="12" t="inlineStr">
-        <is>
-          <t>Actual Date of Completion</t>
-        </is>
-      </c>
-      <c r="O1" s="10" t="inlineStr">
-        <is>
-          <t>Project ID</t>
-        </is>
-      </c>
-      <c r="P1" s="10" t="inlineStr">
-        <is>
-          <t>Contract ID</t>
-        </is>
-      </c>
-      <c r="Q1" s="12" t="inlineStr">
-        <is>
-          <t>Issuance of Invitation to Bid</t>
-        </is>
-      </c>
-      <c r="R1" s="12" t="inlineStr">
-        <is>
-          <t>Pre-Submission Conference</t>
-        </is>
-      </c>
-      <c r="S1" s="12" t="inlineStr">
-        <is>
-          <t>Bid Opening</t>
-        </is>
-      </c>
-      <c r="T1" s="12" t="inlineStr">
-        <is>
-          <t>Issuance of Resolution to Award</t>
-        </is>
-      </c>
-      <c r="U1" s="12" t="inlineStr">
-        <is>
-          <t>Issuance of Notice to Proceed</t>
-        </is>
-      </c>
-      <c r="V1" s="10" t="inlineStr">
-        <is>
-          <t>Name of Contractor</t>
-        </is>
-      </c>
-      <c r="W1" s="10" t="inlineStr">
-        <is>
-          <t>Other Remarks</t>
-        </is>
-      </c>
-      <c r="X1" s="13" t="inlineStr">
-        <is>
-          <t>No. of Sites Reverted</t>
-        </is>
-      </c>
-      <c r="Y1" s="13" t="inlineStr">
-        <is>
-          <t>No. of Sites Not yet started</t>
-        </is>
-      </c>
-      <c r="Z1" s="13" t="inlineStr">
-        <is>
-          <t>No. of Sites Under Procurement</t>
-        </is>
-      </c>
-      <c r="AA1" s="13" t="inlineStr">
-        <is>
-          <t>No. of Sites On Going</t>
-        </is>
-      </c>
-      <c r="AB1" s="13" t="inlineStr">
-        <is>
-          <t>No. of Sites Completed</t>
-        </is>
-      </c>
-      <c r="AC1" s="14" t="inlineStr">
-        <is>
-          <t>PREVIOUS ACCOMPLISHMENT</t>
-        </is>
-      </c>
-      <c r="AD1" s="14" t="inlineStr">
-        <is>
-          <t>DIFFERENCE</t>
-        </is>
-      </c>
-      <c r="AE1" s="13" t="inlineStr">
-        <is>
-          <t>Projected Date of Completion</t>
-        </is>
-      </c>
-      <c r="AF1" s="15" t="inlineStr">
-        <is>
-          <t>Month Completed</t>
-        </is>
-      </c>
-      <c r="AG1" s="6" t="inlineStr">
-        <is>
-          <t>Municipality Classification</t>
-        </is>
+    <row r="1" spans="1:23" s="13" customFormat="1" ht="60.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="2" ht="154.5" customFormat="1" customHeight="1" s="18">
-      <c r="A2" s="20" t="inlineStr">
-        <is>
-          <t>CARAGA</t>
-        </is>
-      </c>
-      <c r="B2" s="20" t="inlineStr">
-        <is>
-          <t>Agusan del Norte</t>
-        </is>
-      </c>
-      <c r="C2" s="20" t="n">
+    <row r="2" spans="1:23" s="14" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="16">
         <v>131508</v>
       </c>
-      <c r="D2" s="20" t="inlineStr">
-        <is>
-          <t>Buenavista CES</t>
-        </is>
-      </c>
-      <c r="E2" s="20" t="inlineStr">
-        <is>
-          <t>BUENAVISTA</t>
-        </is>
-      </c>
-      <c r="F2" s="20" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
-      <c r="G2" s="21" t="n">
+      <c r="D2" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="17">
         <v>1</v>
       </c>
-      <c r="H2" s="20" t="inlineStr">
-        <is>
-          <t>CONSTRUCTION OF TWO (2) STOREY ALTERNATIVE LEARNING SYSTEM - COMMUNITY LEARNING CENTER WITH ROOF DECK- (18.00m x 9.50m), WITH RAINWATER COLLECTOR, PERIMETER FENCE AND FURNITURE</t>
-        </is>
-      </c>
-      <c r="I2" s="22" t="n">
-        <v>14141414.14</v>
-      </c>
-      <c r="J2" s="23" t="n">
+      <c r="H2" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="18">
+        <v>14141414.140000001</v>
+      </c>
+      <c r="J2" s="19">
         <v>14070707.07</v>
       </c>
-      <c r="K2" s="20" t="inlineStr">
-        <is>
-          <t>completed</t>
-        </is>
-      </c>
-      <c r="L2" s="24" t="n">
+      <c r="K2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="20">
         <v>1</v>
       </c>
-      <c r="M2" s="25" t="inlineStr">
-        <is>
-          <t>April 26, 2025</t>
-        </is>
-      </c>
-      <c r="N2" s="25" t="inlineStr">
-        <is>
-          <t>May 15, 2025</t>
-        </is>
-      </c>
-      <c r="O2" s="20" t="inlineStr">
-        <is>
-          <t>ALS-CLC 2024 - CARAGA - AGUSAN DEL NORTE - 001</t>
-        </is>
-      </c>
-      <c r="P2" s="20" t="inlineStr">
-        <is>
-          <t>ALS-CLC 2024 - CARAGA - AGUSAN DEL NORTE - 001</t>
-        </is>
-      </c>
-      <c r="Q2" s="25" t="inlineStr">
-        <is>
-          <t>June 5, 2024</t>
-        </is>
-      </c>
-      <c r="R2" s="25" t="inlineStr">
-        <is>
-          <t>June 28, 2024</t>
-        </is>
-      </c>
-      <c r="S2" s="25" t="inlineStr">
-        <is>
-          <t>July 11, 2024</t>
-        </is>
-      </c>
-      <c r="T2" s="25" t="inlineStr">
-        <is>
-          <t>August 5, 2024</t>
-        </is>
-      </c>
-      <c r="U2" s="25" t="inlineStr">
-        <is>
-          <t>August 15, 2024</t>
-        </is>
-      </c>
-      <c r="V2" s="20" t="inlineStr">
-        <is>
-          <t>JD-RG Const. &amp; Supplies</t>
-        </is>
-      </c>
-      <c r="W2" s="20" t="inlineStr">
-        <is>
-          <t>WITH VARIATION ORDER AND TIME EXTENSION</t>
-        </is>
-      </c>
-      <c r="X2" s="17">
-        <f>IF($K2="Reverted",G2,0)</f>
-        <v/>
-      </c>
-      <c r="Y2" s="17">
-        <f>IF($K2="Not yet started",G2,0)</f>
-        <v/>
-      </c>
-      <c r="Z2" s="17">
-        <f>IF($K2="Under Procurement",G2,0)</f>
-        <v/>
-      </c>
-      <c r="AA2" s="17">
-        <f>IF($K2="Ongoing",G2,0)</f>
-        <v/>
-      </c>
-      <c r="AB2" s="17">
-        <f>IF($K2="Completed",G2,0)</f>
-        <v/>
-      </c>
-      <c r="AC2" s="24" t="n">
+      <c r="M2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" s="14" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="16">
+        <v>100684</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="17">
         <v>1</v>
       </c>
-      <c r="AD2" s="26">
-        <f>L2-AC2</f>
-        <v/>
-      </c>
-      <c r="AE2" s="20" t="n"/>
-      <c r="AF2" s="20" t="n">
-        <v>4.25</v>
-      </c>
-      <c r="AG2" s="20" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
+      <c r="H3" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="18">
+        <v>12871493.449999999</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="20">
+        <v>0.8</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="21"/>
+      <c r="O3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="V3" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="W3" s="16" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="3" ht="154.5" customFormat="1" customHeight="1" s="18">
-      <c r="A3" s="20" t="inlineStr">
-        <is>
-          <t>Region I</t>
-        </is>
-      </c>
-      <c r="B3" s="20" t="inlineStr">
-        <is>
-          <t>Ilocos Sur</t>
-        </is>
-      </c>
-      <c r="C3" s="20" t="n">
-        <v>100684</v>
-      </c>
-      <c r="D3" s="20" t="inlineStr">
-        <is>
-          <t>Sta. Cruz CS</t>
-        </is>
-      </c>
-      <c r="E3" s="20" t="inlineStr">
-        <is>
-          <t>SANTA CRUZ</t>
-        </is>
-      </c>
-      <c r="F3" s="20" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
-      <c r="G3" s="21" t="n">
+    <row r="4" spans="1:23" s="14" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="16">
+        <v>300690</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="17">
         <v>1</v>
       </c>
-      <c r="H3" s="20" t="inlineStr">
-        <is>
-          <t>PROPOSED TWO (2) - STOREY ALTERNATIVE LEARNING SYSTEM (ALS) BUILDING (22.50m x 9.50m) - with Roof Deck</t>
-        </is>
-      </c>
-      <c r="I3" s="22" t="n">
-        <v>12871493.45</v>
-      </c>
-      <c r="J3" s="23" t="inlineStr">
-        <is>
-          <t>Original: 9,322,239.10
-Revised: Php 10,250,272.33</t>
-        </is>
-      </c>
-      <c r="K3" s="20" t="inlineStr">
-        <is>
-          <t>ongoing</t>
-        </is>
-      </c>
-      <c r="L3" s="24" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="M3" s="25" t="inlineStr">
-        <is>
-          <t>Original: 4/18/2025
-Revised: 5/18/2025</t>
-        </is>
-      </c>
-      <c r="N3" s="25" t="n"/>
-      <c r="O3" s="20" t="inlineStr">
-        <is>
-          <t>PB-015-2024</t>
-        </is>
-      </c>
-      <c r="P3" s="20" t="inlineStr">
-        <is>
-          <t>n/a</t>
-        </is>
-      </c>
-      <c r="Q3" s="25" t="inlineStr">
-        <is>
-          <t>October 2, 2024</t>
-        </is>
-      </c>
-      <c r="R3" s="25" t="inlineStr">
-        <is>
-          <t>October 9, 2024</t>
-        </is>
-      </c>
-      <c r="S3" s="25" t="inlineStr">
-        <is>
-          <t>October 22, 2024</t>
-        </is>
-      </c>
-      <c r="T3" s="25" t="inlineStr">
-        <is>
-          <t>October 30, 2024</t>
-        </is>
-      </c>
-      <c r="U3" s="25" t="inlineStr">
-        <is>
-          <t>November 20, 2024</t>
-        </is>
-      </c>
-      <c r="V3" s="20" t="inlineStr">
-        <is>
-          <t>MA Tejada COnstruction</t>
-        </is>
-      </c>
-      <c r="W3" s="20" t="inlineStr">
-        <is>
-          <t>With additional works amounting to Php 928,033.23 due to revision of plans</t>
-        </is>
-      </c>
-      <c r="X3" s="17">
-        <f>IF($K3="Reverted",G3,0)</f>
-        <v/>
-      </c>
-      <c r="Y3" s="17">
-        <f>IF($K3="Not yet started",G3,0)</f>
-        <v/>
-      </c>
-      <c r="Z3" s="17">
-        <f>IF($K3="Under Procurement",G3,0)</f>
-        <v/>
-      </c>
-      <c r="AA3" s="17">
-        <f>IF($K3="Ongoing",G3,0)</f>
-        <v/>
-      </c>
-      <c r="AB3" s="17">
-        <f>IF($K3="Completed",G3,0)</f>
-        <v/>
-      </c>
-      <c r="AC3" s="24" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="AD3" s="26">
-        <f>L3-AC3</f>
-        <v/>
-      </c>
-      <c r="AE3" s="20" t="n"/>
-      <c r="AF3" s="20" t="n"/>
-      <c r="AG3" s="20" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
+      <c r="H4" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="18">
+        <v>12446387.1</v>
+      </c>
+      <c r="J4" s="19">
+        <v>10458975.449999999</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="20">
+        <v>0.7</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="N4" s="21"/>
+      <c r="O4" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q4" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="R4" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="S4" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="T4" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="U4" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="V4" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="W4" s="16" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="4" ht="154.5" customFormat="1" customHeight="1" s="18">
-      <c r="A4" s="20" t="inlineStr">
-        <is>
-          <t>Region III</t>
-        </is>
-      </c>
-      <c r="B4" s="20" t="inlineStr">
-        <is>
-          <t>Aurora</t>
-        </is>
-      </c>
-      <c r="C4" s="20" t="n">
-        <v>300690</v>
-      </c>
-      <c r="D4" s="20" t="inlineStr">
-        <is>
-          <t>Lual NHS</t>
-        </is>
-      </c>
-      <c r="E4" s="20" t="inlineStr">
-        <is>
-          <t>CASIGURAN</t>
-        </is>
-      </c>
-      <c r="F4" s="20" t="inlineStr">
-        <is>
-          <t>Lone</t>
-        </is>
-      </c>
-      <c r="G4" s="21" t="n">
+    <row r="5" spans="1:23" s="14" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="16">
+        <v>301596</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="17">
         <v>1</v>
       </c>
-      <c r="H4" s="20" t="inlineStr">
-        <is>
-          <t>PROPOSED TWO (2) - STOREY ALTERNATIVE LEARNING SYSTEM (ALS) BUILDING (22.50m x 9.50m) - with Roof Deck( TO be elevated by 1.0m)</t>
-        </is>
-      </c>
-      <c r="I4" s="22" t="n">
-        <v>12446387.1</v>
-      </c>
-      <c r="J4" s="23" t="n">
-        <v>10458975.45</v>
-      </c>
-      <c r="K4" s="20" t="inlineStr">
-        <is>
-          <t>ongoing</t>
-        </is>
-      </c>
-      <c r="L4" s="24" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="M4" s="25" t="inlineStr">
-        <is>
-          <t>June 21, 2025</t>
-        </is>
-      </c>
-      <c r="N4" s="25" t="n"/>
-      <c r="O4" s="20" t="inlineStr">
-        <is>
-          <t>2024-04-181</t>
-        </is>
-      </c>
-      <c r="P4" s="20" t="inlineStr">
-        <is>
-          <t>SGOD-INFRA-32</t>
-        </is>
-      </c>
-      <c r="Q4" s="25" t="inlineStr">
-        <is>
-          <t>July 1, 2024</t>
-        </is>
-      </c>
-      <c r="R4" s="25" t="inlineStr">
-        <is>
-          <t>July 8, 2024</t>
-        </is>
-      </c>
-      <c r="S4" s="25" t="inlineStr">
-        <is>
-          <t>July 22, 2024</t>
-        </is>
-      </c>
-      <c r="T4" s="25" t="inlineStr">
-        <is>
-          <t>August 1, 2024</t>
-        </is>
-      </c>
-      <c r="U4" s="25" t="inlineStr">
-        <is>
-          <t>August 17, 2024</t>
-        </is>
-      </c>
-      <c r="V4" s="20" t="inlineStr">
-        <is>
-          <t>MACCO CONSTRUCTION</t>
-        </is>
-      </c>
-      <c r="W4" s="20" t="inlineStr">
-        <is>
-          <t>Request to utilized savings is up to now no response from CO</t>
-        </is>
-      </c>
-      <c r="X4" s="17">
-        <f>IF($K4="Reverted",G4,0)</f>
-        <v/>
-      </c>
-      <c r="Y4" s="17">
-        <f>IF($K4="Not yet started",G4,0)</f>
-        <v/>
-      </c>
-      <c r="Z4" s="17">
-        <f>IF($K4="Under Procurement",G4,0)</f>
-        <v/>
-      </c>
-      <c r="AA4" s="17">
-        <f>IF($K4="Ongoing",G4,0)</f>
-        <v/>
-      </c>
-      <c r="AB4" s="17">
-        <f>IF($K4="Completed",G4,0)</f>
-        <v/>
-      </c>
-      <c r="AC4" s="24" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AD4" s="26">
-        <f>L4-AC4</f>
-        <v/>
-      </c>
-      <c r="AE4" s="20" t="n"/>
-      <c r="AF4" s="20" t="n"/>
-      <c r="AG4" s="20" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="154.5" customFormat="1" customHeight="1" s="18">
-      <c r="A5" s="20" t="inlineStr">
-        <is>
-          <t>Region IV-B</t>
-        </is>
-      </c>
-      <c r="B5" s="20" t="inlineStr">
-        <is>
-          <t>Occidental Mindoro</t>
-        </is>
-      </c>
-      <c r="C5" s="20" t="n">
-        <v>301596</v>
-      </c>
-      <c r="D5" s="20" t="inlineStr">
-        <is>
-          <t>Sablayan National Comprehensive High School</t>
-        </is>
-      </c>
-      <c r="E5" s="20" t="inlineStr">
-        <is>
-          <t>SABLAYAN</t>
-        </is>
-      </c>
-      <c r="F5" s="20" t="inlineStr">
-        <is>
-          <t>Lone</t>
-        </is>
-      </c>
-      <c r="G5" s="21" t="n">
+      <c r="H5" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="18">
+        <v>16540705.310000001</v>
+      </c>
+      <c r="J5" s="19">
+        <v>16458637.91</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="20">
         <v>1</v>
       </c>
-      <c r="H5" s="20" t="inlineStr">
-        <is>
-          <t>PROPOSED TWO (2) - STOREY ALTERNATIVE LEARNING SYSTEM (ALS) BUILDING (22.50m x 9.50m) - with Roof Deck</t>
-        </is>
-      </c>
-      <c r="I5" s="22" t="n">
-        <v>16540705.31</v>
-      </c>
-      <c r="J5" s="23" t="n">
-        <v>16458637.91</v>
-      </c>
-      <c r="K5" s="20" t="inlineStr">
-        <is>
-          <t>completed</t>
-        </is>
-      </c>
-      <c r="L5" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" s="25" t="inlineStr">
-        <is>
-          <t>April 10, 2025</t>
-        </is>
-      </c>
-      <c r="N5" s="25" t="inlineStr">
-        <is>
-          <t>April 15,2025</t>
-        </is>
-      </c>
-      <c r="O5" s="20" t="inlineStr">
-        <is>
-          <t>DepEd-OccMdo-2024-05</t>
-        </is>
-      </c>
-      <c r="P5" s="20" t="n"/>
-      <c r="Q5" s="25" t="inlineStr">
-        <is>
-          <t>May 31, 2024</t>
-        </is>
-      </c>
-      <c r="R5" s="25" t="inlineStr">
-        <is>
-          <t>June 10 2024</t>
-        </is>
-      </c>
-      <c r="S5" s="25" t="inlineStr">
-        <is>
-          <t>June 24, 2024</t>
-        </is>
-      </c>
-      <c r="T5" s="25" t="inlineStr">
-        <is>
-          <t>June 28, 2024</t>
-        </is>
-      </c>
-      <c r="U5" s="25" t="inlineStr">
-        <is>
-          <t>June 19, 2024</t>
-        </is>
-      </c>
-      <c r="V5" s="20" t="inlineStr">
-        <is>
-          <t>hawkstow construction and development</t>
-        </is>
-      </c>
-      <c r="W5" s="20" t="inlineStr">
-        <is>
-          <t>actual target completion was adjusted due to contractor request for extension regarding weather condition</t>
-        </is>
-      </c>
-      <c r="X5" s="17">
-        <f>IF($K5="Reverted",G5,0)</f>
-        <v/>
-      </c>
-      <c r="Y5" s="17">
-        <f>IF($K5="Not yet started",G5,0)</f>
-        <v/>
-      </c>
-      <c r="Z5" s="17">
-        <f>IF($K5="Under Procurement",G5,0)</f>
-        <v/>
-      </c>
-      <c r="AA5" s="17">
-        <f>IF($K5="Ongoing",G5,0)</f>
-        <v/>
-      </c>
-      <c r="AB5" s="17">
-        <f>IF($K5="Completed",G5,0)</f>
-        <v/>
-      </c>
-      <c r="AC5" s="24" t="n">
-        <v>0.83</v>
-      </c>
-      <c r="AD5" s="26">
-        <f>L5-AC5</f>
-        <v/>
-      </c>
-      <c r="AE5" s="20" t="n"/>
-      <c r="AF5" s="20" t="n"/>
-      <c r="AG5" s="20" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
+      <c r="M5" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="R5" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="S5" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="T5" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="V5" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="W5" s="16" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AI5"/>
+  <autoFilter ref="A1:W5" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="C1:C2 C4 C6:C1048576">
-    <cfRule type="duplicateValues" priority="5" dxfId="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="duplicateValues" priority="3" dxfId="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="duplicateValues" priority="4" dxfId="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:W5">
-    <cfRule type="containsBlanks" priority="1" dxfId="0">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(J2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC5">
-    <cfRule type="containsBlanks" priority="2" dxfId="0">
-      <formula>LEN(TRIM(AC2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" paperSize="9" scale="51"/>
+  <pageSetup paperSize="9" scale="51" orientation="landscape"/>
 </worksheet>
 </file>
</xml_diff>